<commit_message>
C+- corrigido e backup taylor 2GHz sincronizado
</commit_message>
<xml_diff>
--- a/Resultados Multicore.xlsx
+++ b/Resultados Multicore.xlsx
@@ -277,7 +277,7 @@
     <t xml:space="preserve">20(2)</t>
   </si>
   <si>
-    <t xml:space="preserve">21(12)</t>
+    <t xml:space="preserve">21(4)</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -943,8 +943,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="28070936"/>
-        <c:axId val="44516588"/>
+        <c:axId val="91008961"/>
+        <c:axId val="37478212"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1207,11 +1207,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="38418977"/>
-        <c:axId val="13537390"/>
+        <c:axId val="14811437"/>
+        <c:axId val="11638567"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28070936"/>
+        <c:axId val="91008961"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1277,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44516588"/>
+        <c:crossAx val="37478212"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44516588"/>
+        <c:axId val="37478212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1368,13 +1368,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28070936"/>
+        <c:crossAx val="91008961"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="38418977"/>
+        <c:axId val="14811437"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,14 +1406,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13537390"/>
+        <c:crossAx val="11638567"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13537390"/>
+        <c:axId val="11638567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,8 +1449,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.932684442990349"/>
-              <c:y val="0.0678326636728906"/>
+              <c:x val="0.932663234452889"/>
+              <c:y val="0.0676043020919513"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1484,7 +1484,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38418977"/>
+        <c:crossAx val="14811437"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -1547,7 +1547,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1773,8 +1773,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="96657017"/>
-        <c:axId val="96363087"/>
+        <c:axId val="71347837"/>
+        <c:axId val="5366730"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2001,11 +2001,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="48343479"/>
-        <c:axId val="80046700"/>
+        <c:axId val="64045010"/>
+        <c:axId val="32947993"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96657017"/>
+        <c:axId val="71347837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2071,7 +2071,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96363087"/>
+        <c:crossAx val="5366730"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2079,7 +2079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96363087"/>
+        <c:axId val="5366730"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,13 +2162,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96657017"/>
+        <c:crossAx val="71347837"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10000"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="48343479"/>
+        <c:axId val="64045010"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,14 +2200,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80046700"/>
+        <c:crossAx val="32947993"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80046700"/>
+        <c:axId val="32947993"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2270,7 +2270,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48343479"/>
+        <c:crossAx val="64045010"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -2333,7 +2333,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2518,11 +2518,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="76109786"/>
-        <c:axId val="40153922"/>
+        <c:axId val="48181803"/>
+        <c:axId val="45689125"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76109786"/>
+        <c:axId val="48181803"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2590,7 +2590,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40153922"/>
+        <c:crossAx val="45689125"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2598,7 +2598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40153922"/>
+        <c:axId val="45689125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2681,7 +2681,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76109786"/>
+        <c:crossAx val="48181803"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2711,7 +2711,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2932,11 +2932,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="68773756"/>
-        <c:axId val="61127793"/>
+        <c:axId val="62603721"/>
+        <c:axId val="76537442"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68773756"/>
+        <c:axId val="62603721"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3004,7 +3004,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61127793"/>
+        <c:crossAx val="76537442"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3012,7 +3012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61127793"/>
+        <c:axId val="76537442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3095,7 +3095,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68773756"/>
+        <c:crossAx val="62603721"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3123,7 +3123,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3349,8 +3349,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="74408961"/>
-        <c:axId val="63221396"/>
+        <c:axId val="62297466"/>
+        <c:axId val="46338492"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3577,11 +3577,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="51936416"/>
-        <c:axId val="60842291"/>
+        <c:axId val="76883409"/>
+        <c:axId val="50020654"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74408961"/>
+        <c:axId val="62297466"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3647,7 +3647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63221396"/>
+        <c:crossAx val="46338492"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3655,7 +3655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63221396"/>
+        <c:axId val="46338492"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3738,12 +3738,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74408961"/>
+        <c:crossAx val="62297466"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="51936416"/>
+        <c:axId val="76883409"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3775,14 +3775,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60842291"/>
+        <c:crossAx val="50020654"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60842291"/>
+        <c:axId val="50020654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3818,8 +3818,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.932671924022725"/>
-              <c:y val="0.0677945907303705"/>
+              <c:x val="0.932649949169773"/>
+              <c:y val="0.0675643469971401"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3853,7 +3853,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51936416"/>
+        <c:crossAx val="76883409"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3915,7 +3915,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4141,8 +4141,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="56913557"/>
-        <c:axId val="34427402"/>
+        <c:axId val="72487722"/>
+        <c:axId val="28803578"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4405,11 +4405,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="48607344"/>
-        <c:axId val="40118534"/>
+        <c:axId val="96186709"/>
+        <c:axId val="47707695"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56913557"/>
+        <c:axId val="72487722"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4475,7 +4475,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34427402"/>
+        <c:crossAx val="28803578"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4483,7 +4483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34427402"/>
+        <c:axId val="28803578"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4566,12 +4566,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56913557"/>
+        <c:crossAx val="72487722"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="48607344"/>
+        <c:axId val="96186709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4603,14 +4603,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40118534"/>
+        <c:crossAx val="47707695"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40118534"/>
+        <c:axId val="47707695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4673,7 +4673,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48607344"/>
+        <c:crossAx val="96186709"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4735,7 +4735,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4956,11 +4956,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="85852624"/>
-        <c:axId val="57214327"/>
+        <c:axId val="53645054"/>
+        <c:axId val="37027378"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85852624"/>
+        <c:axId val="53645054"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,7 +5028,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57214327"/>
+        <c:crossAx val="37027378"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5036,7 +5036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57214327"/>
+        <c:axId val="37027378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5119,7 +5119,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85852624"/>
+        <c:crossAx val="53645054"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5147,7 +5147,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5373,8 +5373,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="74912351"/>
-        <c:axId val="46369197"/>
+        <c:axId val="44593404"/>
+        <c:axId val="53710011"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5601,11 +5601,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="45820289"/>
-        <c:axId val="5162466"/>
+        <c:axId val="11882890"/>
+        <c:axId val="56795227"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74912351"/>
+        <c:axId val="44593404"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5671,7 +5671,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46369197"/>
+        <c:crossAx val="53710011"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5679,7 +5679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46369197"/>
+        <c:axId val="53710011"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5762,12 +5762,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74912351"/>
+        <c:crossAx val="44593404"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="45820289"/>
+        <c:axId val="11882890"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5799,14 +5799,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5162466"/>
+        <c:crossAx val="56795227"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5162466"/>
+        <c:axId val="56795227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5842,8 +5842,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.93267763269459"/>
-              <c:y val="0.0677945907303705"/>
+              <c:x val="0.932661358631204"/>
+              <c:y val="0.0675643469971401"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5877,7 +5877,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45820289"/>
+        <c:crossAx val="11882890"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5939,7 +5939,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6165,8 +6165,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="61042488"/>
-        <c:axId val="97490976"/>
+        <c:axId val="81090190"/>
+        <c:axId val="70926375"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6429,11 +6429,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="22708362"/>
-        <c:axId val="1548012"/>
+        <c:axId val="22649284"/>
+        <c:axId val="71701219"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61042488"/>
+        <c:axId val="81090190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6499,7 +6499,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97490976"/>
+        <c:crossAx val="70926375"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6507,7 +6507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97490976"/>
+        <c:axId val="70926375"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6590,12 +6590,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61042488"/>
+        <c:crossAx val="81090190"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="22708362"/>
+        <c:axId val="22649284"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6627,14 +6627,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1548012"/>
+        <c:crossAx val="71701219"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1548012"/>
+        <c:axId val="71701219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6697,7 +6697,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22708362"/>
+        <c:crossAx val="22649284"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6759,7 +6759,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6980,11 +6980,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="79819668"/>
-        <c:axId val="63684723"/>
+        <c:axId val="8168800"/>
+        <c:axId val="68702193"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79819668"/>
+        <c:axId val="8168800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7052,7 +7052,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63684723"/>
+        <c:crossAx val="68702193"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7060,7 +7060,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63684723"/>
+        <c:axId val="68702193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7143,7 +7143,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79819668"/>
+        <c:crossAx val="8168800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7171,7 +7171,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7397,8 +7397,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="36292610"/>
-        <c:axId val="66916125"/>
+        <c:axId val="13742825"/>
+        <c:axId val="54270548"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7625,11 +7625,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="53148098"/>
-        <c:axId val="74944309"/>
+        <c:axId val="48420810"/>
+        <c:axId val="13215352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36292610"/>
+        <c:axId val="13742825"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7695,7 +7695,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66916125"/>
+        <c:crossAx val="54270548"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7703,7 +7703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66916125"/>
+        <c:axId val="54270548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7786,12 +7786,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36292610"/>
+        <c:crossAx val="13742825"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="53148098"/>
+        <c:axId val="48420810"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7823,14 +7823,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74944309"/>
+        <c:crossAx val="13215352"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74944309"/>
+        <c:axId val="13215352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7866,8 +7866,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.93267763269459"/>
-              <c:y val="0.0676754438222328"/>
+              <c:x val="0.932661358631204"/>
+              <c:y val="0.0674451858913251"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -7901,7 +7901,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53148098"/>
+        <c:crossAx val="48420810"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7963,7 +7963,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8117,68 +8117,8 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="1">
-                  <c:v>69307</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>59442</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>52108</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48214</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44546</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>40811</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>38346</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>35872</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>34653</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32362</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>31148</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>29882</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>28627</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>28640</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27477</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>26206</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>26212</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>24972</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>24983</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>23697</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>23676</c:v>
+                  <c:v>23810</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8186,8 +8126,8 @@
         </c:ser>
         <c:gapWidth val="247"/>
         <c:overlap val="0"/>
-        <c:axId val="40190793"/>
-        <c:axId val="28942013"/>
+        <c:axId val="70025098"/>
+        <c:axId val="84299406"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8371,66 +8311,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="1">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>112</c:v>
-                </c:pt>
                 <c:pt idx="21">
                   <c:v>112</c:v>
                 </c:pt>
@@ -8447,11 +8327,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="97226232"/>
-        <c:axId val="65907723"/>
+        <c:axId val="7206594"/>
+        <c:axId val="46437200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40190793"/>
+        <c:axId val="70025098"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8517,7 +8397,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28942013"/>
+        <c:crossAx val="84299406"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8525,7 +8405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28942013"/>
+        <c:axId val="84299406"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8608,12 +8488,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40190793"/>
+        <c:crossAx val="70025098"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="97226232"/>
+        <c:axId val="7206594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8645,14 +8525,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65907723"/>
+        <c:crossAx val="46437200"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65907723"/>
+        <c:axId val="46437200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8715,7 +8595,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97226232"/>
+        <c:crossAx val="7206594"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8777,7 +8657,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8919,68 +8799,8 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="1">
-                  <c:v>513822</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>450450</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>401676</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>372360</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>351648</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>326706</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>313248</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>297270</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>294756</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>274833</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>269334</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>262725</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>255096</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>263736</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>254472</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>244398</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>251658</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>240219</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>246834</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>234180</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>236580</c:v>
+                  <c:v>259280</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8995,11 +8815,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="2655234"/>
-        <c:axId val="81796697"/>
+        <c:axId val="23455176"/>
+        <c:axId val="71451243"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2655234"/>
+        <c:axId val="23455176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9067,7 +8887,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81796697"/>
+        <c:crossAx val="71451243"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9075,7 +8895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81796697"/>
+        <c:axId val="71451243"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9158,7 +8978,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2655234"/>
+        <c:crossAx val="23455176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9197,9 +9017,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>141480</xdr:colOff>
+      <xdr:colOff>141120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9207,8 +9027,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13889160" y="47520"/>
-        <a:ext cx="4401000" cy="3045960"/>
+        <a:off x="13889880" y="47520"/>
+        <a:ext cx="4404960" cy="3045600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9227,9 +9047,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>426960</xdr:colOff>
+      <xdr:colOff>426600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9237,8 +9057,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13873320" y="2931120"/>
-        <a:ext cx="4702320" cy="3014640"/>
+        <a:off x="13874040" y="2931120"/>
+        <a:ext cx="4706280" cy="3014280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9257,9 +9077,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>458640</xdr:colOff>
+      <xdr:colOff>458280</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9267,8 +9087,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="18403200" y="79200"/>
-        <a:ext cx="3328560" cy="2696760"/>
+        <a:off x="18408240" y="79200"/>
+        <a:ext cx="3328560" cy="2696400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9287,9 +9107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>599760</xdr:colOff>
+      <xdr:colOff>599400</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>137520</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9297,8 +9117,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="18710640" y="2628720"/>
-        <a:ext cx="4392720" cy="3017880"/>
+        <a:off x="18715680" y="2628720"/>
+        <a:ext cx="4394160" cy="3017520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9322,9 +9142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>503640</xdr:colOff>
+      <xdr:colOff>503280</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9332,8 +9152,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17569080" y="170280"/>
-        <a:ext cx="4245120" cy="3021120"/>
+        <a:off x="17574840" y="170280"/>
+        <a:ext cx="4249080" cy="3020760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9352,9 +9172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>453240</xdr:colOff>
+      <xdr:colOff>452880</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9362,8 +9182,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12898080" y="45360"/>
-        <a:ext cx="4558320" cy="3014280"/>
+        <a:off x="12900600" y="45360"/>
+        <a:ext cx="4561200" cy="3013920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9382,9 +9202,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>588240</xdr:colOff>
+      <xdr:colOff>587880</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9392,8 +9212,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21981240" y="156240"/>
-        <a:ext cx="4224600" cy="2755080"/>
+        <a:off x="21992040" y="156240"/>
+        <a:ext cx="4228200" cy="2754720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9417,9 +9237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>504360</xdr:colOff>
+      <xdr:colOff>504000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9427,8 +9247,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16787520" y="170280"/>
-        <a:ext cx="4245480" cy="3021120"/>
+        <a:off x="16791120" y="170280"/>
+        <a:ext cx="4249800" cy="3020760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9447,9 +9267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>453240</xdr:colOff>
+      <xdr:colOff>452880</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9458,7 +9278,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12762360" y="45360"/>
-        <a:ext cx="3912480" cy="3014280"/>
+        <a:ext cx="3915720" cy="3013920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9477,9 +9297,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>588600</xdr:colOff>
+      <xdr:colOff>588240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9487,8 +9307,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21199320" y="156240"/>
-        <a:ext cx="4225320" cy="2755080"/>
+        <a:off x="21208320" y="156240"/>
+        <a:ext cx="4228560" cy="2754720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9512,9 +9332,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>504360</xdr:colOff>
+      <xdr:colOff>504000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9522,8 +9342,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16787520" y="170280"/>
-        <a:ext cx="4245480" cy="3021120"/>
+        <a:off x="16791120" y="170280"/>
+        <a:ext cx="4249800" cy="3020760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9542,9 +9362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>453240</xdr:colOff>
+      <xdr:colOff>452880</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9553,7 +9373,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12762360" y="45360"/>
-        <a:ext cx="3912480" cy="3014280"/>
+        <a:ext cx="3915720" cy="3013920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9572,9 +9392,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>588600</xdr:colOff>
+      <xdr:colOff>588240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9582,8 +9402,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="21199320" y="156240"/>
-        <a:ext cx="4225320" cy="2755080"/>
+        <a:off x="21208320" y="156240"/>
+        <a:ext cx="4228560" cy="2754720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9607,7 +9427,7 @@
       <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
@@ -10974,7 +10794,7 @@
       <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.88"/>
@@ -12204,11 +12024,11 @@
       <selection pane="topLeft" activeCell="U23" activeCellId="0" sqref="U23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="6.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="17" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="17" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="13.36"/>
@@ -13432,14 +13252,14 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="7.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="6.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="17" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="17" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="13.36"/>
@@ -13581,15 +13401,9 @@
       <c r="K3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="35" t="n">
-        <v>69307</v>
-      </c>
-      <c r="M3" s="36" t="n">
-        <v>252</v>
-      </c>
-      <c r="N3" s="37" t="n">
-        <v>513822</v>
-      </c>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="37"/>
       <c r="O3" s="17" t="n">
         <f aca="false">F3/1000</f>
         <v>1.4525</v>
@@ -13632,15 +13446,9 @@
       <c r="K4" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="35" t="n">
-        <v>59442</v>
-      </c>
-      <c r="M4" s="36" t="n">
-        <v>252</v>
-      </c>
-      <c r="N4" s="37" t="n">
-        <v>450450</v>
-      </c>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="37"/>
       <c r="O4" s="17" t="n">
         <f aca="false">F4/1000</f>
         <v>1.252484</v>
@@ -13683,15 +13491,9 @@
       <c r="K5" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="35" t="n">
-        <v>52108</v>
-      </c>
-      <c r="M5" s="36" t="n">
-        <v>252</v>
-      </c>
-      <c r="N5" s="37" t="n">
-        <v>401676</v>
-      </c>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="37"/>
       <c r="O5" s="17" t="n">
         <f aca="false">F5/1000</f>
         <v>1.101962</v>
@@ -13734,15 +13536,9 @@
       <c r="K6" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="35" t="n">
-        <v>48214</v>
-      </c>
-      <c r="M6" s="36" t="n">
-        <v>132</v>
-      </c>
-      <c r="N6" s="37" t="n">
-        <v>372360</v>
-      </c>
+      <c r="L6" s="35"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="37"/>
       <c r="O6" s="17" t="n">
         <f aca="false">F6/1000</f>
         <v>1.001883</v>
@@ -13786,15 +13582,9 @@
       <c r="K7" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="35" t="n">
-        <v>44546</v>
-      </c>
-      <c r="M7" s="36" t="n">
-        <v>132</v>
-      </c>
-      <c r="N7" s="37" t="n">
-        <v>351648</v>
-      </c>
+      <c r="L7" s="35"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="37"/>
       <c r="O7" s="17" t="n">
         <f aca="false">F7/1000</f>
         <v>0.926463</v>
@@ -13837,15 +13627,9 @@
       <c r="K8" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="35" t="n">
-        <v>40811</v>
-      </c>
-      <c r="M8" s="36" t="n">
-        <v>132</v>
-      </c>
-      <c r="N8" s="37" t="n">
-        <v>326706</v>
-      </c>
+      <c r="L8" s="35"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="37"/>
       <c r="O8" s="17" t="n">
         <f aca="false">F8/1000</f>
         <v>0.85125</v>
@@ -13888,15 +13672,9 @@
       <c r="K9" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="35" t="n">
-        <v>38346</v>
-      </c>
-      <c r="M9" s="36" t="n">
-        <v>132</v>
-      </c>
-      <c r="N9" s="37" t="n">
-        <v>313248</v>
-      </c>
+      <c r="L9" s="35"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="37"/>
       <c r="O9" s="17" t="n">
         <f aca="false">F9/1000</f>
         <v>0.801585</v>
@@ -13939,15 +13717,9 @@
       <c r="K10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="35" t="n">
-        <v>35872</v>
-      </c>
-      <c r="M10" s="36" t="n">
-        <v>132</v>
-      </c>
-      <c r="N10" s="37" t="n">
-        <v>297270</v>
-      </c>
+      <c r="L10" s="35"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="37"/>
       <c r="O10" s="17" t="n">
         <f aca="false">F10/1000</f>
         <v>0.751282</v>
@@ -13991,15 +13763,9 @@
       <c r="K11" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="35" t="n">
-        <v>34653</v>
-      </c>
-      <c r="M11" s="36" t="n">
-        <v>132</v>
-      </c>
-      <c r="N11" s="37" t="n">
-        <v>294756</v>
-      </c>
+      <c r="L11" s="35"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="37"/>
       <c r="O11" s="17" t="n">
         <f aca="false">F11/1000</f>
         <v>0.72631</v>
@@ -14042,15 +13808,9 @@
       <c r="K12" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="35" t="n">
-        <v>32362</v>
-      </c>
-      <c r="M12" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N12" s="37" t="n">
-        <v>274833</v>
-      </c>
+      <c r="L12" s="35"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="37"/>
       <c r="O12" s="17" t="n">
         <f aca="false">F12/1000</f>
         <v>0.676001</v>
@@ -14093,15 +13853,9 @@
       <c r="K13" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="L13" s="35" t="n">
-        <v>31148</v>
-      </c>
-      <c r="M13" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N13" s="37" t="n">
-        <v>269334</v>
-      </c>
+      <c r="L13" s="35"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="37"/>
       <c r="O13" s="17" t="n">
         <f aca="false">F13/1000</f>
         <v>0.651354</v>
@@ -14144,15 +13898,9 @@
       <c r="K14" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="L14" s="35" t="n">
-        <v>29882</v>
-      </c>
-      <c r="M14" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N14" s="37" t="n">
-        <v>262725</v>
-      </c>
+      <c r="L14" s="35"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="37"/>
       <c r="O14" s="17" t="n">
         <f aca="false">F14/1000</f>
         <v>0.626382</v>
@@ -14195,15 +13943,9 @@
       <c r="K15" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="L15" s="35" t="n">
-        <v>28627</v>
-      </c>
-      <c r="M15" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N15" s="37" t="n">
-        <v>255096</v>
-      </c>
+      <c r="L15" s="35"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="37"/>
       <c r="O15" s="17" t="n">
         <f aca="false">F15/1000</f>
         <v>0.601312</v>
@@ -14247,15 +13989,9 @@
       <c r="K16" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="L16" s="35" t="n">
-        <v>28640</v>
-      </c>
-      <c r="M16" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N16" s="37" t="n">
-        <v>263736</v>
-      </c>
+      <c r="L16" s="35"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="37"/>
       <c r="O16" s="17" t="n">
         <f aca="false">F16/1000</f>
         <v>0.601175</v>
@@ -14299,15 +14035,9 @@
       <c r="K17" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="L17" s="35" t="n">
-        <v>27477</v>
-      </c>
-      <c r="M17" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N17" s="37" t="n">
-        <v>254472</v>
-      </c>
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="37"/>
       <c r="O17" s="17" t="n">
         <f aca="false">F17/1000</f>
         <v>0.57575</v>
@@ -14350,15 +14080,9 @@
       <c r="K18" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="L18" s="35" t="n">
-        <v>26206</v>
-      </c>
-      <c r="M18" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N18" s="37" t="n">
-        <v>244398</v>
-      </c>
+      <c r="L18" s="35"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="17" t="n">
         <f aca="false">F18/1000</f>
         <v>0.550625</v>
@@ -14402,15 +14126,9 @@
       <c r="K19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="L19" s="35" t="n">
-        <v>26212</v>
-      </c>
-      <c r="M19" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N19" s="37" t="n">
-        <v>251658</v>
-      </c>
+      <c r="L19" s="35"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="37"/>
       <c r="O19" s="17" t="n">
         <f aca="false">F19/1000</f>
         <v>0.5513</v>
@@ -14453,15 +14171,9 @@
       <c r="K20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="L20" s="35" t="n">
-        <v>24972</v>
-      </c>
-      <c r="M20" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N20" s="37" t="n">
-        <v>240219</v>
-      </c>
+      <c r="L20" s="35"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="37"/>
       <c r="O20" s="17" t="n">
         <f aca="false">F20/1000</f>
         <v>0.526325</v>
@@ -14505,15 +14217,9 @@
       <c r="K21" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="L21" s="35" t="n">
-        <v>24983</v>
-      </c>
-      <c r="M21" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N21" s="37" t="n">
-        <v>246834</v>
-      </c>
+      <c r="L21" s="35"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="37"/>
       <c r="O21" s="17" t="n">
         <f aca="false">F21/1000</f>
         <v>0.526048</v>
@@ -14557,15 +14263,9 @@
       <c r="K22" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="L22" s="35" t="n">
-        <v>23697</v>
-      </c>
-      <c r="M22" s="36" t="n">
-        <v>112</v>
-      </c>
-      <c r="N22" s="37" t="n">
-        <v>234180</v>
-      </c>
+      <c r="L22" s="35"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="37"/>
       <c r="O22" s="17" t="n">
         <f aca="false">F22/1000</f>
         <v>0.498597</v>
@@ -14610,13 +14310,13 @@
         <v>84</v>
       </c>
       <c r="L23" s="35" t="n">
-        <v>23676</v>
+        <v>23810</v>
       </c>
       <c r="M23" s="36" t="n">
         <v>112</v>
       </c>
       <c r="N23" s="37" t="n">
-        <v>236580</v>
+        <v>259280</v>
       </c>
       <c r="O23" s="17" t="n">
         <f aca="false">F23/1000</f>

</xml_diff>